<commit_message>
PAC Report changes done
</commit_message>
<xml_diff>
--- a/UPPRB_Web/Resource/PAC_Details.xlsx
+++ b/UPPRB_Web/Resource/PAC_Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAD046F-11F8-46B2-AA51-052A193A3D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{4CAD046F-11F8-46B2-AA51-052A193A3D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB1E3635-7ED0-4F66-BBFD-60996B9687AF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PAC Detail" sheetId="7" r:id="rId1"/>
+    <sheet name="PAC Detail" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="AssetGroup">OFFSET(#REF!,0,0,COUNTA(#REF!)-1,1)</definedName>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Created Date</t>
   </si>
@@ -61,9 +61,6 @@
     <t>PS Name</t>
   </si>
   <si>
-    <t>Examine Center Name</t>
-  </si>
-  <si>
     <t>Solver Name</t>
   </si>
   <si>
@@ -86,6 +83,12 @@
   </si>
   <si>
     <t>Cyber Security &amp; Preventive Action Cell (CSPAC) Details</t>
+  </si>
+  <si>
+    <t>Center Name</t>
+  </si>
+  <si>
+    <t>Center Status</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +126,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,16 +168,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -191,23 +201,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>361950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E13DCB96-40A6-CBBF-212D-663F88C0ADE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E7C430A-A58E-4949-8F22-0514C0C03262}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -230,7 +240,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4489450" y="63500"/>
+          <a:off x="3384550" y="88900"/>
           <a:ext cx="5194300" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -549,73 +559,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6959F0D-C72E-4CF9-B52B-9DB1CD705521}">
-  <dimension ref="A1:P3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F344E1C5-676A-4BBC-B8C3-26133AAF8C8A}">
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" customWidth="1"/>
-    <col min="10" max="10" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="18.54296875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="20.36328125" customWidth="1"/>
-    <col min="15" max="15" width="24.1796875" customWidth="1"/>
-    <col min="16" max="16" width="18.26953125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
+    <row r="2" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -638,40 +644,42 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A1:P1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>